<commit_message>
Updated documents, clean up files
</commit_message>
<xml_diff>
--- a/ベースマシン・パラメータ一覧.xlsx
+++ b/ベースマシン・パラメータ一覧.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
   <si>
     <t>ベースマシン・パラメータ一覧</t>
     <rPh sb="12" eb="14">
@@ -25,22 +25,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>2016.11.20</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Oscillator</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Filter</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Amp</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>WaveShape</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -78,10 +66,6 @@
   </si>
   <si>
     <t>Name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Type</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -196,14 +180,66 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>2016.12.19</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Envelope</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0..Length</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0..Length</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>音符の持続時間(Tickカウント)</t>
+    <rPh sb="0" eb="2">
+      <t>オンプ</t>
+    </rPh>
+    <rPh sb="3" eb="7">
+      <t>ジゾクジカン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Decayの持続時間(Tickカウント)</t>
+    <rPh sb="6" eb="10">
+      <t>ジゾクジカン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Sustainレベル</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Oscillator</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>0..4095</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>再考</t>
-    <rPh sb="0" eb="2">
-      <t>サイコウ</t>
-    </rPh>
+    <t>ノートの長さ（Tickカウント) =BPM120の4分音符(Sampling Rate = 1ms)</t>
+    <rPh sb="4" eb="5">
+      <t>ナガ</t>
+    </rPh>
+    <rPh sb="25" eb="29">
+      <t>シブオンプ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Attackレベル</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -211,7 +247,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,6 +260,15 @@
       <sz val="6"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
@@ -250,8 +295,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -550,7 +598,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -560,203 +610,216 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1">
+      <c r="A4" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
         <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="1" customFormat="1">
+      <c r="A10" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="1" customFormat="1">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="1" customFormat="1">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="1" customFormat="1">
+      <c r="A16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" t="s">
-        <v>28</v>
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>125</v>
+      </c>
+      <c r="D18" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="D20" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>